<commit_message>
Initial commit - Detection Of Multiple Pension Schemes
</commit_message>
<xml_diff>
--- a/suspicious_clusters_report.xlsx
+++ b/suspicious_clusters_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,193 +467,193 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>16180.72</v>
+        <v>40617.33</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E2" t="n">
         <v>-1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.615</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>11838.07</v>
+        <v>46440.69</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E3" t="n">
         <v>-1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.395</v>
+        <v>0.9500000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>30491.29</v>
+        <v>33532.21</v>
       </c>
       <c r="D4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
         <v>-1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.99</v>
+        <v>0.821875</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>23205.17</v>
+        <v>8027.79</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>-1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9099999999999999</v>
+        <v>0.215625</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>10489.88</v>
+        <v>29952.92</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E6" t="n">
         <v>-1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.405</v>
+        <v>0.7875</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>7826.25</v>
+        <v>26792.33</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E7" t="n">
         <v>-1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.175</v>
+        <v>0.6687500000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>16189.63</v>
+        <v>7697.42</v>
       </c>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
         <v>-1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.71</v>
+        <v>0.371875</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>2482.48</v>
+        <v>11287.01</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
         <v>-1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.125</v>
+        <v>0.246875</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>18233.32</v>
+        <v>11664.86</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
         <v>-1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.715</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>13780.14</v>
+        <v>13238.11</v>
       </c>
       <c r="D11" t="n">
         <v>3</v>
@@ -662,7 +662,127 @@
         <v>-1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.46</v>
+        <v>0.340625</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>97</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>26064.56</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.665625</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>126</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2482.48</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.096875</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>156</v>
+      </c>
+      <c r="B14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" t="n">
+        <v>32901.47</v>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.74375</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>157</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>12578.63</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.253125</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>158</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" t="n">
+        <v>28672.08</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5906250000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>159</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>21572.56</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.409375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>